<commit_message>
Add list of variables
</commit_message>
<xml_diff>
--- a/Questions/Example_Questions.xlsx
+++ b/Questions/Example_Questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fernunich-my.sharepoint.com/personal/michael_rihs_fernuni_ch/Documents/Dokumente/Programming/Pool_Tool/Questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{33B8347F-231F-4540-B4F4-A461C7C25E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D5A14DB-19EA-624D-AD69-D2CE71204BC5}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="8_{33B8347F-231F-4540-B4F4-A461C7C25E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{379349AD-6F1C-1D42-A21F-C4EDE3BB9875}"/>
   <bookViews>
-    <workbookView xWindow="-74880" yWindow="2700" windowWidth="28240" windowHeight="17240" xr2:uid="{B03B835C-97AF-C440-9EDB-ED73ED60FD46}"/>
+    <workbookView xWindow="-74880" yWindow="2700" windowWidth="31420" windowHeight="17240" xr2:uid="{B03B835C-97AF-C440-9EDB-ED73ED60FD46}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
-  <si>
-    <t>Question_ID</t>
-  </si>
-  <si>
-    <t>Questiontype</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
   <si>
     <t>Question</t>
   </si>
@@ -161,12 +155,6 @@
     <t>Wien</t>
   </si>
   <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>False</t>
-  </si>
-  <si>
     <t>Welche Länder liegen in Europa?</t>
   </si>
   <si>
@@ -209,10 +197,46 @@
     <t>D_cor</t>
   </si>
   <si>
-    <t>ß</t>
-  </si>
-  <si>
-    <t>A_Cor</t>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>A_type_cor</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>Chapter</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Finalized</t>
+  </si>
+  <si>
+    <t>Creating</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -601,305 +625,411 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{307D6B60-4F12-3548-8BE6-74749C19A1E2}">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="13.1640625" customWidth="1"/>
-    <col min="3" max="3" width="55.1640625" customWidth="1"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" customWidth="1"/>
+    <col min="3" max="3" width="5.5" customWidth="1"/>
+    <col min="4" max="4" width="55.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>61</v>
+      </c>
+      <c r="R1" t="s">
+        <v>58</v>
+      </c>
+      <c r="S1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="O2">
+        <v>2024</v>
+      </c>
+      <c r="P2">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3">
+        <v>2024</v>
+      </c>
+      <c r="P3">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L1" t="s">
-        <v>55</v>
-      </c>
-      <c r="M1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4">
+        <v>2024</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+      <c r="Q4">
+        <v>3</v>
+      </c>
+      <c r="R4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5">
+        <v>2024</v>
+      </c>
+      <c r="P5">
+        <v>3</v>
+      </c>
+      <c r="Q5">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="R5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="I6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O6">
+        <v>2024</v>
+      </c>
+      <c r="P6">
+        <v>4</v>
+      </c>
+      <c r="Q6">
+        <v>5</v>
+      </c>
+      <c r="R6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" t="s">
         <v>37</v>
       </c>
-      <c r="D7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="H7" t="s">
         <v>38</v>
       </c>
-      <c r="F7" t="s">
+      <c r="K7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L7" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N7" t="s">
+        <v>54</v>
+      </c>
+      <c r="O7">
+        <v>2024</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G7" t="s">
+      <c r="E8" t="s">
         <v>40</v>
       </c>
-      <c r="J7" t="s">
+      <c r="F8" t="s">
         <v>41</v>
       </c>
-      <c r="K7" t="s">
-        <v>41</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="G8" t="s">
         <v>42</v>
       </c>
-      <c r="M7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="H8" t="s">
         <v>43</v>
       </c>
-      <c r="D8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" t="s">
-        <v>47</v>
-      </c>
-      <c r="J8" t="s">
-        <v>41</v>
-      </c>
       <c r="K8" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="L8" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="M8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+      <c r="N8" t="s">
+        <v>53</v>
+      </c>
+      <c r="O8">
+        <v>2024</v>
+      </c>
+      <c r="P8">
+        <v>2</v>
+      </c>
+      <c r="Q8">
+        <v>2</v>
+      </c>
+      <c r="R8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F29" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
+      <c r="B30" s="1"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="I30" s="2"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F30" s="2"/>
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
-      <c r="B31" s="2"/>
+      <c r="B31" s="1"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
-      <c r="I31" s="2"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F31" s="2"/>
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
-      <c r="B32" s="2"/>
+      <c r="B32" s="1"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
-      <c r="I32" s="2"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F32" s="2"/>
+      <c r="J32" s="2"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
-      <c r="B33" s="2"/>
+      <c r="B33" s="1"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
-      <c r="I33" s="2"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F33" s="2"/>
+      <c r="J33" s="2"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
-      <c r="B34" s="2"/>
+      <c r="B34" s="1"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
-      <c r="I34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="J34" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add function to update input
</commit_message>
<xml_diff>
--- a/Questions/Example_Questions.xlsx
+++ b/Questions/Example_Questions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fernunich-my.sharepoint.com/personal/michael_rihs_fernuni_ch/Documents/Dokumente/Programming/Pool_Tool/Questions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelrihs/Fernuni/Programming/Pool_Tool/Questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="128" documentId="8_{33B8347F-231F-4540-B4F4-A461C7C25E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CFEB0616-6FA7-3B4B-86C4-0D71BCD44937}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1488C556-BA14-434F-AB41-883D4B1E8211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" xr2:uid="{B03B835C-97AF-C440-9EDB-ED73ED60FD46}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
   <si>
     <t>Question</t>
   </si>
@@ -114,18 +114,6 @@
   </si>
   <si>
     <t>Welches dieser Elemente ist ein Edelgas?</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
   </si>
   <si>
     <t>A</t>
@@ -636,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{307D6B60-4F12-3548-8BE6-74749C19A1E2}">
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -650,64 +638,64 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" t="s">
         <v>45</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>46</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
         <v>53</v>
       </c>
-      <c r="K1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L1" t="s">
-        <v>50</v>
-      </c>
-      <c r="M1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R1" t="s">
         <v>52</v>
       </c>
-      <c r="O1" t="s">
-        <v>57</v>
-      </c>
-      <c r="P1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>59</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>56</v>
       </c>
-      <c r="S1" t="s">
-        <v>60</v>
-      </c>
       <c r="T1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -718,7 +706,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>22</v>
@@ -736,7 +724,7 @@
         <v>5</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="J2" t="s">
         <v>26</v>
@@ -752,7 +740,7 @@
         <v>1</v>
       </c>
       <c r="R2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -763,7 +751,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>23</v>
@@ -781,7 +769,7 @@
         <v>9</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="J3" t="s">
         <v>26</v>
@@ -796,7 +784,7 @@
         <v>2</v>
       </c>
       <c r="R3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
@@ -807,10 +795,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>10</v>
@@ -825,10 +813,10 @@
         <v>13</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="O4">
         <v>2024</v>
@@ -840,7 +828,7 @@
         <v>3</v>
       </c>
       <c r="R4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
@@ -851,7 +839,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>24</v>
@@ -869,10 +857,10 @@
         <v>17</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J5" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="O5">
         <v>2024</v>
@@ -884,7 +872,7 @@
         <v>4</v>
       </c>
       <c r="R5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
@@ -895,7 +883,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>25</v>
@@ -916,7 +904,7 @@
         <v>19</v>
       </c>
       <c r="J6" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="O6">
         <v>2024</v>
@@ -928,7 +916,7 @@
         <v>5</v>
       </c>
       <c r="R6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
@@ -942,31 +930,31 @@
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="K7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="N7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="O7">
         <v>2024</v>
@@ -978,7 +966,7 @@
         <v>1</v>
       </c>
       <c r="R7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
@@ -992,31 +980,31 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" t="s">
         <v>39</v>
       </c>
-      <c r="E8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" t="s">
-        <v>43</v>
-      </c>
       <c r="K8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="M8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="N8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="O8">
         <v>2024</v>
@@ -1028,7 +1016,7 @@
         <v>2</v>
       </c>
       <c r="R8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Improve display of current questions
</commit_message>
<xml_diff>
--- a/Questions/Example_Questions.xlsx
+++ b/Questions/Example_Questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelrihs/Fernuni/Programming/Pool_Tool/Questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1488C556-BA14-434F-AB41-883D4B1E8211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1255AF-78AF-C84A-8AB4-7657612734BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" xr2:uid="{B03B835C-97AF-C440-9EDB-ED73ED60FD46}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
   <si>
     <t>Question</t>
   </si>
@@ -207,9 +207,6 @@
   </si>
   <si>
     <t>Tags</t>
-  </si>
-  <si>
-    <t>Finalized</t>
   </si>
   <si>
     <t>Creating</t>
@@ -625,7 +622,7 @@
   <dimension ref="A1:T34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,7 +641,7 @@
         <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -695,7 +692,7 @@
         <v>56</v>
       </c>
       <c r="T1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -740,7 +737,7 @@
         <v>1</v>
       </c>
       <c r="R2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -784,7 +781,7 @@
         <v>2</v>
       </c>
       <c r="R3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
@@ -828,7 +825,7 @@
         <v>3</v>
       </c>
       <c r="R4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
@@ -916,7 +913,7 @@
         <v>5</v>
       </c>
       <c r="R6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
@@ -945,16 +942,16 @@
         <v>34</v>
       </c>
       <c r="K7" t="s">
+        <v>60</v>
+      </c>
+      <c r="L7" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" t="s">
         <v>61</v>
       </c>
-      <c r="L7" t="s">
+      <c r="N7" t="s">
         <v>61</v>
-      </c>
-      <c r="M7" t="s">
-        <v>62</v>
-      </c>
-      <c r="N7" t="s">
-        <v>62</v>
       </c>
       <c r="O7">
         <v>2024</v>
@@ -966,7 +963,7 @@
         <v>1</v>
       </c>
       <c r="R7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
@@ -995,16 +992,16 @@
         <v>39</v>
       </c>
       <c r="K8" t="s">
+        <v>60</v>
+      </c>
+      <c r="L8" t="s">
         <v>61</v>
       </c>
-      <c r="L8" t="s">
-        <v>62</v>
-      </c>
       <c r="M8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O8">
         <v>2024</v>
@@ -1016,7 +1013,7 @@
         <v>2</v>
       </c>
       <c r="R8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Sort Data on load
</commit_message>
<xml_diff>
--- a/Questions/Example_Questions.xlsx
+++ b/Questions/Example_Questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelrihs/Fernuni/Programming/Pool_Tool/Questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1255AF-78AF-C84A-8AB4-7657612734BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D5B877-C6A0-7542-ACE8-C5F015139F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" xr2:uid="{B03B835C-97AF-C440-9EDB-ED73ED60FD46}"/>
   </bookViews>
@@ -621,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{307D6B60-4F12-3548-8BE6-74749C19A1E2}">
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -778,7 +778,7 @@
         <v>2</v>
       </c>
       <c r="Q3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="R3" t="s">
         <v>57</v>

</xml_diff>